<commit_message>
Esquema de barras modificado
</commit_message>
<xml_diff>
--- a/Documentos/Calculo posiciones.xlsx
+++ b/Documentos/Calculo posiciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALVARO\UPM\4. Cuarto de carrera\Segundo cuatri\TFG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BF85DC-9D6B-4354-BBAB-BD3F8F58258A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACD3187-0C58-4EA0-A6F2-CC882B439901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A4E45D7-FABD-4DA9-B739-54C29D37A65E}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{7A4E45D7-FABD-4DA9-B739-54C29D37A65E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="39">
   <si>
     <t>desplazamiento</t>
   </si>
@@ -147,14 +147,21 @@
   </si>
   <si>
     <t>l7</t>
+  </si>
+  <si>
+    <t>prx</t>
+  </si>
+  <si>
+    <t>alpha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -213,7 +220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -231,6 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -566,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3F29D36-5D76-4C29-8778-65CB13092E3D}">
-  <dimension ref="A2:AB16"/>
+  <dimension ref="A2:AD16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF5" sqref="AF5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,7 +585,7 @@
     <col min="2" max="21" width="8.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>18</v>
       </c>
@@ -614,7 +622,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" s="7" t="s">
         <v>0</v>
@@ -666,7 +674,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" t="s">
         <v>2</v>
@@ -742,7 +750,7 @@
         <v>0.21213203435596426</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -827,7 +835,7 @@
         <v>-3.6126080441681698</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
@@ -903,7 +911,7 @@
         <v>6.8000000000000005E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -978,7 +986,7 @@
         <v>0.23599999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -1054,8 +1062,26 @@
       <c r="X8">
         <v>1.49E-2</v>
       </c>
+      <c r="Z8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2</v>
+      </c>
       <c r="B9">
         <f>X6/2</f>
         <v>3.4000000000000002E-2</v>
@@ -1093,15 +1119,15 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <f>X7-H9-$X$16</f>
+        <f>X7-H10-$X$16</f>
         <v>0.22399999999999998</v>
       </c>
       <c r="N9">
         <v>0</v>
       </c>
       <c r="O9">
-        <f>-X8+H9+$X$16</f>
-        <v>-2.8999999999999998E-3</v>
+        <f>-X8+$X$16</f>
+        <v>-1.29E-2</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1127,8 +1153,26 @@
       <c r="X9">
         <v>0.28000000000000003</v>
       </c>
+      <c r="Z9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <f>X13/2 - X13/4</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AC9" s="9">
+        <f>AB9*COS(AA9)</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AD9" s="9">
+        <f>AB9*SIN(AA9)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1167,8 +1211,7 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <f>H10+$X$16</f>
-        <v>1.2E-2</v>
+        <v>0</v>
       </c>
       <c r="M10">
         <f>X9-H10-$X$16</f>
@@ -1178,8 +1221,8 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <f>X10-H10-$X$16</f>
-        <v>9.9999999999999985E-3</v>
+        <f>X10-$X$16</f>
+        <v>1.9999999999999997E-2</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1205,8 +1248,27 @@
       <c r="X10">
         <v>2.1999999999999999E-2</v>
       </c>
+      <c r="Z10">
+        <v>2</v>
+      </c>
+      <c r="AA10">
+        <f>AA9+120</f>
+        <v>120</v>
+      </c>
+      <c r="AB10">
+        <f>AB9</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AC10" s="9">
+        <f>-AB10*COS(AA10)</f>
+        <v>-2.0354524263164045E-2</v>
+      </c>
+      <c r="AD10" s="9">
+        <f>AB10*SIN(AA10)</f>
+        <v>1.4515279605307858E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1281,8 +1343,27 @@
       <c r="X11">
         <v>8.6999999999999994E-2</v>
       </c>
+      <c r="Z11">
+        <v>3</v>
+      </c>
+      <c r="AA11">
+        <f>AA10+120</f>
+        <v>240</v>
+      </c>
+      <c r="AB11">
+        <f>AB10</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AC11" s="9">
+        <f>-AB11*COS(AA11)</f>
+        <v>-8.1445326383787035E-3</v>
+      </c>
+      <c r="AD11" s="9">
+        <f>-AB11*SIN(AA11)</f>
+        <v>-2.363612887302792E-2</v>
+      </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>5</v>
       </c>
@@ -1357,13 +1438,13 @@
         <v>6.8000000000000005E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
       <c r="B13">
-        <f>X12/2+X14</f>
-        <v>5.4000000000000006E-2</v>
+        <f>X12/2+X14/2</f>
+        <v>4.4000000000000004E-2</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1432,7 +1513,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="W14" t="s">
         <v>31</v>
       </c>
@@ -1440,7 +1521,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="W16" t="s">
         <v>33</v>
       </c>

</xml_diff>